<commit_message>
Añade clear secret button
</commit_message>
<xml_diff>
--- a/server/temp/secret-shares.xlsx
+++ b/server/temp/secret-shares.xlsx
@@ -79,7 +79,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1325624</v>
+        <v>27446547</v>
       </c>
     </row>
     <row r="3">
@@ -87,7 +87,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>23884200</v>
+        <v>11284996</v>
       </c>
     </row>
     <row r="4">
@@ -95,7 +95,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>31811262</v>
+        <v>27237078</v>
       </c>
     </row>
     <row r="5">
@@ -103,7 +103,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>25420356</v>
+        <v>7025799</v>
       </c>
     </row>
     <row r="6">
@@ -111,7 +111,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>15515620</v>
+        <v>12207958</v>
       </c>
     </row>
     <row r="7">
@@ -119,7 +119,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>23391784</v>
+        <v>32847345</v>
       </c>
     </row>
     <row r="8">
@@ -127,7 +127,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>13725236</v>
+        <v>21069208</v>
       </c>
     </row>
     <row r="9">
@@ -135,7 +135,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>28791890</v>
+        <v>25278121</v>
       </c>
     </row>
     <row r="10">
@@ -143,7 +143,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>20694851</v>
+        <v>22385649</v>
       </c>
     </row>
     <row r="11">
@@ -151,7 +151,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>19136750</v>
+        <v>18473749</v>
       </c>
     </row>
     <row r="12">
@@ -159,7 +159,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>30756343</v>
+        <v>15240303</v>
       </c>
     </row>
     <row r="13">
@@ -167,7 +167,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>5574044</v>
+        <v>9999118</v>
       </c>
     </row>
     <row r="14">
@@ -175,7 +175,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>4764260</v>
+        <v>29234393</v>
       </c>
     </row>
     <row r="15">
@@ -183,7 +183,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>32883056</v>
+        <v>27937318</v>
       </c>
     </row>
     <row r="16">
@@ -191,7 +191,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>4313688</v>
+        <v>23823942</v>
       </c>
     </row>
     <row r="17">
@@ -199,7 +199,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>11702339</v>
+        <v>30226239</v>
       </c>
     </row>
     <row r="18">
@@ -207,7 +207,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>23967916</v>
+        <v>22537641</v>
       </c>
     </row>
     <row r="19">
@@ -215,7 +215,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>20519918</v>
+        <v>5321972</v>
       </c>
     </row>
     <row r="20">
@@ -223,7 +223,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>24812903</v>
+        <v>12313448</v>
       </c>
     </row>
     <row r="21">
@@ -231,7 +231,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>3683087</v>
+        <v>5753276</v>
       </c>
     </row>
     <row r="22">
@@ -239,7 +239,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>1566212</v>
+        <v>10607522</v>
       </c>
     </row>
     <row r="23">
@@ -247,7 +247,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>6279678</v>
+        <v>13903710</v>
       </c>
     </row>
     <row r="24">
@@ -255,7 +255,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>16131477</v>
+        <v>31839756</v>
       </c>
     </row>
     <row r="25">
@@ -263,7 +263,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>6365726</v>
+        <v>9120567</v>
       </c>
     </row>
     <row r="26">
@@ -271,7 +271,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>29826068</v>
+        <v>20284843</v>
       </c>
     </row>
     <row r="27">
@@ -279,7 +279,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>15628870</v>
+        <v>1269341</v>
       </c>
     </row>
     <row r="28">
@@ -287,7 +287,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>4044492</v>
+        <v>17844611</v>
       </c>
     </row>
     <row r="29">
@@ -295,7 +295,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>12279419</v>
+        <v>30733727</v>
       </c>
     </row>
     <row r="30">
@@ -303,7 +303,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>921794</v>
+        <v>29830155</v>
       </c>
     </row>
     <row r="31">
@@ -311,7 +311,87 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>8159286</v>
+        <v>643286</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>24961837</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>12418115</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>2478220</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>30224177</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>25690535</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>15191169</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>20655879</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>26075923</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>11058484</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>17935604</v>
       </c>
     </row>
   </sheetData>

</xml_diff>